<commit_message>
critical exponents calculation and record OK
</commit_message>
<xml_diff>
--- a/Planilhas de análise/Controle.xlsx
+++ b/Planilhas de análise/Controle.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="881" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="881"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,6 @@
     <definedName name="propano_exp_1" localSheetId="2">Propano!$E$4:$F$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36231,43 +36230,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36275,7 +36274,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36303,7 +36302,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36571,8 +36570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37654,7 +37653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+    <sheetView topLeftCell="G34" workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Renormalization - Binary Mixture OK
</commit_message>
<xml_diff>
--- a/Planilhas de análise/Controle.xlsx
+++ b/Planilhas de análise/Controle.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="881" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="881" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="1" r:id="rId1"/>
@@ -40263,27 +40263,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="propano_exp" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="propano_exp_1" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="propano_exp" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octano_exp" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_exp3_near" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40555,8 +40555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47227,8 +47227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59521,8 +59521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>